<commit_message>
KNN class structure update
</commit_message>
<xml_diff>
--- a/predictions/predictions.xlsx
+++ b/predictions/predictions.xlsx
@@ -1296,7 +1296,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -2556,7 +2556,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4851,7 +4851,7 @@
       </c>
       <c r="K98" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -5121,7 +5121,7 @@
       </c>
       <c r="K104" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6246,7 +6246,7 @@
       </c>
       <c r="K129" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6966,7 +6966,7 @@
       </c>
       <c r="K145" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -7956,7 +7956,7 @@
       </c>
       <c r="K167" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9621,7 +9621,7 @@
       </c>
       <c r="K204" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13896,7 +13896,7 @@
       </c>
       <c r="K299" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -14391,7 +14391,7 @@
       </c>
       <c r="K310" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -14751,7 +14751,7 @@
       </c>
       <c r="K318" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -16011,7 +16011,7 @@
       </c>
       <c r="K346" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -18621,7 +18621,7 @@
       </c>
       <c r="K404" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -20601,7 +20601,7 @@
       </c>
       <c r="K448" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21231,7 +21231,7 @@
       </c>
       <c r="K462" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -25056,7 +25056,7 @@
       </c>
       <c r="K547" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -26451,7 +26451,7 @@
       </c>
       <c r="K578" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -28071,7 +28071,7 @@
       </c>
       <c r="K614" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -29421,7 +29421,7 @@
       </c>
       <c r="K644" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -29556,7 +29556,7 @@
       </c>
       <c r="K647" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -29871,7 +29871,7 @@
       </c>
       <c r="K654" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -31491,7 +31491,7 @@
       </c>
       <c r="K690" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -33201,7 +33201,7 @@
       </c>
       <c r="K728" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -34506,7 +34506,7 @@
       </c>
       <c r="K757" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -36981,7 +36981,7 @@
       </c>
       <c r="K812" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -37611,7 +37611,7 @@
       </c>
       <c r="K826" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -38556,7 +38556,7 @@
       </c>
       <c r="K847" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -39141,7 +39141,7 @@
       </c>
       <c r="K860" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -41706,7 +41706,7 @@
       </c>
       <c r="K917" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -42201,7 +42201,7 @@
       </c>
       <c r="K928" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -43326,7 +43326,7 @@
       </c>
       <c r="K953" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -45171,7 +45171,7 @@
       </c>
       <c r="K994" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
some comments, and some negative progress (plotter) bruh
</commit_message>
<xml_diff>
--- a/predictions/predictions.xlsx
+++ b/predictions/predictions.xlsx
@@ -1296,7 +1296,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5121,7 +5121,7 @@
       </c>
       <c r="K104" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -6246,7 +6246,7 @@
       </c>
       <c r="K129" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -6426,7 +6426,7 @@
       </c>
       <c r="K133" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6696,7 +6696,7 @@
       </c>
       <c r="K139" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6966,7 +6966,7 @@
       </c>
       <c r="K145" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7281,7 +7281,7 @@
       </c>
       <c r="K152" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -7956,7 +7956,7 @@
       </c>
       <c r="K167" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -8451,7 +8451,7 @@
       </c>
       <c r="K178" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9621,7 +9621,7 @@
       </c>
       <c r="K204" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -10746,7 +10746,7 @@
       </c>
       <c r="K229" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -11826,7 +11826,7 @@
       </c>
       <c r="K253" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -12816,7 +12816,7 @@
       </c>
       <c r="K275" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13896,7 +13896,7 @@
       </c>
       <c r="K299" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14211,7 +14211,7 @@
       </c>
       <c r="K306" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14391,7 +14391,7 @@
       </c>
       <c r="K310" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14751,7 +14751,7 @@
       </c>
       <c r="K318" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14931,7 +14931,7 @@
       </c>
       <c r="K322" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -15291,7 +15291,7 @@
       </c>
       <c r="K330" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -15426,7 +15426,7 @@
       </c>
       <c r="K333" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -17181,7 +17181,7 @@
       </c>
       <c r="K372" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -20601,7 +20601,7 @@
       </c>
       <c r="K448" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -21231,7 +21231,7 @@
       </c>
       <c r="K462" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -25056,7 +25056,7 @@
       </c>
       <c r="K547" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -25731,7 +25731,7 @@
       </c>
       <c r="K562" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -26451,7 +26451,7 @@
       </c>
       <c r="K578" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -28656,7 +28656,7 @@
       </c>
       <c r="K627" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -29421,7 +29421,7 @@
       </c>
       <c r="K644" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -29556,7 +29556,7 @@
       </c>
       <c r="K647" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -29871,7 +29871,7 @@
       </c>
       <c r="K654" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -31491,7 +31491,7 @@
       </c>
       <c r="K690" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -32661,7 +32661,7 @@
       </c>
       <c r="K716" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -33201,7 +33201,7 @@
       </c>
       <c r="K728" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -33696,7 +33696,7 @@
       </c>
       <c r="K739" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -37161,7 +37161,7 @@
       </c>
       <c r="K816" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -37611,7 +37611,7 @@
       </c>
       <c r="K826" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -38556,7 +38556,7 @@
       </c>
       <c r="K847" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -41706,7 +41706,7 @@
       </c>
       <c r="K917" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -43821,7 +43821,7 @@
       </c>
       <c r="K964" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -44136,7 +44136,7 @@
       </c>
       <c r="K971" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>

</xml_diff>